<commit_message>
change in SH code
</commit_message>
<xml_diff>
--- a/storage/app/excels/ncm.xlsx
+++ b/storage/app/excels/ncm.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24228"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\hd-v2\storage\app\excels\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\www\hd-v2\storage\app\excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{500E9822-EBF1-4CD0-8989-FCF76F335FC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="85">
   <si>
     <t>Description (English)</t>
   </si>
@@ -80,18 +81,6 @@
     <t>400129</t>
   </si>
   <si>
-    <t>Book &amp; Collections</t>
-  </si>
-  <si>
-    <t>Livro e coleções</t>
-  </si>
-  <si>
-    <t>Libro y colecciones</t>
-  </si>
-  <si>
-    <t>490700</t>
-  </si>
-  <si>
     <t>Cameras</t>
   </si>
   <si>
@@ -282,13 +271,22 @@
   </si>
   <si>
     <t>Ereaders | Lector de libros digitales</t>
+  </si>
+  <si>
+    <t>Books, Newspapers or Magazines</t>
+  </si>
+  <si>
+    <t>Libros, periódicos o revistas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Livros, Jornais ou Revistas </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -309,6 +307,18 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10.5"/>
+      <color rgb="FF1F497D"/>
+      <name val="Century Gothic"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -331,7 +341,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -347,6 +357,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -626,14 +640,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:D27"/>
+  <dimension ref="A1:F27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -644,7 +658,7 @@
     <col min="4" max="4" width="23.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -658,7 +672,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -672,7 +686,7 @@
         <v>610190</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -686,7 +700,7 @@
         <v>854231</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -700,7 +714,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -714,183 +728,184 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="D6" s="3">
+        <v>490199</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>18</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B7" t="s">
         <v>19</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C7" t="s">
         <v>20</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D7" s="3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>22</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B8" t="s">
         <v>23</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C8" t="s">
         <v>24</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>26</v>
-      </c>
-      <c r="B8" t="s">
-        <v>27</v>
-      </c>
-      <c r="C8" t="s">
-        <v>28</v>
       </c>
       <c r="D8" s="3">
         <v>847170</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" t="s">
+        <v>27</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F9" s="8"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>29</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B10" t="s">
         <v>30</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C10" t="s">
+        <v>30</v>
+      </c>
+      <c r="D10" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="D9" s="3" t="s">
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="B11" t="s">
         <v>33</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C11" t="s">
         <v>34</v>
       </c>
-      <c r="C10" t="s">
-        <v>34</v>
-      </c>
-      <c r="D10" s="3" t="s">
+      <c r="D11" s="3" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>36</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B12" t="s">
         <v>37</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C12" t="s">
         <v>38</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>40</v>
-      </c>
-      <c r="B12" t="s">
-        <v>41</v>
-      </c>
-      <c r="C12" t="s">
-        <v>42</v>
       </c>
       <c r="D12" s="3">
         <v>210610</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>39</v>
+      </c>
+      <c r="B13" t="s">
+        <v>40</v>
+      </c>
+      <c r="C13" t="s">
+        <v>41</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>43</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B14" t="s">
         <v>44</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C14" t="s">
         <v>45</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>47</v>
-      </c>
-      <c r="B14" t="s">
-        <v>48</v>
-      </c>
-      <c r="C14" t="s">
-        <v>49</v>
       </c>
       <c r="D14" s="3">
         <v>392690</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>46</v>
+      </c>
+      <c r="B15" t="s">
+        <v>47</v>
+      </c>
+      <c r="C15" t="s">
+        <v>48</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>50</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B16" t="s">
         <v>51</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C16" t="s">
+        <v>51</v>
+      </c>
+      <c r="D16" s="3" t="s">
         <v>52</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>54</v>
-      </c>
-      <c r="B16" t="s">
-        <v>55</v>
-      </c>
-      <c r="C16" t="s">
-        <v>55</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B17" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="C17" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B18" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C18" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="D18" s="3">
         <v>630790</v>
@@ -898,27 +913,27 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B19" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="C19" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="D20" s="5">
         <v>621139</v>
@@ -926,13 +941,13 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B21" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="C21" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="D21" s="3">
         <v>847130</v>
@@ -940,27 +955,27 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="B22" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C22" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B23" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="C23" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="D23" s="3">
         <v>300450</v>
@@ -968,16 +983,16 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="B24" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="C24" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -1010,13 +1025,13 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="B27" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="D27" s="3">
         <v>854370</v>

</xml_diff>

<commit_message>
change in model deposit order status
</commit_message>
<xml_diff>
--- a/storage/app/excels/ncm.xlsx
+++ b/storage/app/excels/ncm.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24228"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\hd-v2\storage\app\excels\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\www\hd-v2\storage\app\excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{500E9822-EBF1-4CD0-8989-FCF76F335FC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="85">
   <si>
     <t>Description (English)</t>
   </si>
@@ -80,18 +81,6 @@
     <t>400129</t>
   </si>
   <si>
-    <t>Book &amp; Collections</t>
-  </si>
-  <si>
-    <t>Livro e coleções</t>
-  </si>
-  <si>
-    <t>Libro y colecciones</t>
-  </si>
-  <si>
-    <t>490700</t>
-  </si>
-  <si>
     <t>Cameras</t>
   </si>
   <si>
@@ -282,13 +271,22 @@
   </si>
   <si>
     <t>Ereaders | Lector de libros digitales</t>
+  </si>
+  <si>
+    <t>Books, Newspapers or Magazines</t>
+  </si>
+  <si>
+    <t>Libros, periódicos o revistas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Livros, Jornais ou Revistas </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -309,6 +307,18 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10.5"/>
+      <color rgb="FF1F497D"/>
+      <name val="Century Gothic"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -331,7 +341,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -347,6 +357,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -626,14 +640,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:D27"/>
+  <dimension ref="A1:F27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -644,7 +658,7 @@
     <col min="4" max="4" width="23.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -658,7 +672,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -672,7 +686,7 @@
         <v>610190</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -686,7 +700,7 @@
         <v>854231</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -700,7 +714,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -714,183 +728,184 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="D6" s="3">
+        <v>490199</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>18</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B7" t="s">
         <v>19</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C7" t="s">
         <v>20</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D7" s="3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>22</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B8" t="s">
         <v>23</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C8" t="s">
         <v>24</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>26</v>
-      </c>
-      <c r="B8" t="s">
-        <v>27</v>
-      </c>
-      <c r="C8" t="s">
-        <v>28</v>
       </c>
       <c r="D8" s="3">
         <v>847170</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" t="s">
+        <v>27</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F9" s="8"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>29</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B10" t="s">
         <v>30</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C10" t="s">
+        <v>30</v>
+      </c>
+      <c r="D10" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="D9" s="3" t="s">
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="B11" t="s">
         <v>33</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C11" t="s">
         <v>34</v>
       </c>
-      <c r="C10" t="s">
-        <v>34</v>
-      </c>
-      <c r="D10" s="3" t="s">
+      <c r="D11" s="3" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>36</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B12" t="s">
         <v>37</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C12" t="s">
         <v>38</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>40</v>
-      </c>
-      <c r="B12" t="s">
-        <v>41</v>
-      </c>
-      <c r="C12" t="s">
-        <v>42</v>
       </c>
       <c r="D12" s="3">
         <v>210610</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>39</v>
+      </c>
+      <c r="B13" t="s">
+        <v>40</v>
+      </c>
+      <c r="C13" t="s">
+        <v>41</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>43</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B14" t="s">
         <v>44</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C14" t="s">
         <v>45</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>47</v>
-      </c>
-      <c r="B14" t="s">
-        <v>48</v>
-      </c>
-      <c r="C14" t="s">
-        <v>49</v>
       </c>
       <c r="D14" s="3">
         <v>392690</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>46</v>
+      </c>
+      <c r="B15" t="s">
+        <v>47</v>
+      </c>
+      <c r="C15" t="s">
+        <v>48</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>50</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B16" t="s">
         <v>51</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C16" t="s">
+        <v>51</v>
+      </c>
+      <c r="D16" s="3" t="s">
         <v>52</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>54</v>
-      </c>
-      <c r="B16" t="s">
-        <v>55</v>
-      </c>
-      <c r="C16" t="s">
-        <v>55</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B17" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="C17" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B18" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C18" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="D18" s="3">
         <v>630790</v>
@@ -898,27 +913,27 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B19" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="C19" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="D20" s="5">
         <v>621139</v>
@@ -926,13 +941,13 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B21" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="C21" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="D21" s="3">
         <v>847130</v>
@@ -940,27 +955,27 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="B22" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C22" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B23" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="C23" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="D23" s="3">
         <v>300450</v>
@@ -968,16 +983,16 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="B24" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="C24" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -1010,13 +1025,13 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="B27" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="D27" s="3">
         <v>854370</v>

</xml_diff>